<commit_message>
Updated flux meta data after level one raise in july 2020
</commit_message>
<xml_diff>
--- a/metadata/flux_metadata_level1_15min.xlsx
+++ b/metadata/flux_metadata_level1_15min.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867FAAFD-7FEA-9548-86A2-69D24FD3E16F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C479CF-C047-6F4D-9335-01776CD25B12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28780" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43420" yWindow="-1520" windowWidth="23440" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global-attributes" sheetId="1" r:id="rId1"/>
@@ -209,9 +209,6 @@
   </si>
   <si>
     <t>15 minutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Platform height is the top of the Met tower, sensor height is plaform height minus 12.5 m. 10 Hz sampling rate on both licor and sonic. Runs 15 mins in length. Run time stamp: start of run. </t>
   </si>
   <si>
     <t>sonic - 0111117433, Gas analyser - 75H-0800</t>
@@ -268,6 +265,9 @@
   </si>
   <si>
     <t>timeSeries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platform height is the top of the Met tower, sensor height is plaform height minus 10.87 m. 10 Hz sampling rate on both licor and sonic. Runs 15 mins in length. Run time stamp: start of run. </t>
   </si>
 </sst>
 </file>
@@ -710,7 +710,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -733,7 +733,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -741,7 +741,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -765,7 +765,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -773,7 +773,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -781,7 +781,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -821,7 +821,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -845,7 +845,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -853,7 +853,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -885,7 +885,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -939,7 +939,7 @@
         <v>30</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -979,7 +979,7 @@
         <v>37</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -999,7 +999,7 @@
         <v>40</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -1042,7 +1042,7 @@
         <v>44</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>